<commit_message>
Complete Phase 1+2 Tables List and Select Star
</commit_message>
<xml_diff>
--- a/SIF_select_only/Tables-List.xlsx
+++ b/SIF_select_only/Tables-List.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://data3-my.sharepoint.com/personal/philip_antrobus_businessaspect_com_au/Documents/Documents/GitHub/AU-SIF-SQL/SIF_select_only/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD9FC62-7F28-4A74-87F1-DF151013C91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{5FD9FC62-7F28-4A74-87F1-DF151013C91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{267F888F-0B85-49C9-AD6A-B854C3D216FB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{938F974C-F50E-4B13-AC4E-C8E52C2D0EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables-List" sheetId="2" r:id="rId1"/>
+    <sheet name="PivotTable" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tables-List'!$A$1:$G$267</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tables-List'!$A$1:$H$266</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="301">
   <si>
     <t>TableName</t>
   </si>
@@ -977,7 +981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -994,6 +998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,6 +1014,2966 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Philip Antrobus" refreshedDate="45905.302953587961" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="265" xr:uid="{5BEDD449-7DBB-4ADE-A7AF-E0E87C190FB7}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:H266" sheet="Tables-List"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Create Table Order" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="265"/>
+    </cacheField>
+    <cacheField name="TableName" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Mapped Yet?" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Group" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="27" count="28">
+        <n v="0"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="13"/>
+        <n v="14"/>
+        <n v="15"/>
+        <n v="16"/>
+        <n v="17"/>
+        <n v="18"/>
+        <n v="19"/>
+        <n v="20"/>
+        <n v="21"/>
+        <n v="22"/>
+        <n v="23"/>
+        <n v="24"/>
+        <n v="25"/>
+        <n v="26"/>
+        <n v="27"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Area" numFmtId="0">
+      <sharedItems count="28">
+        <s v="Tables populated by SIF specification"/>
+        <s v="eMinerva sourced reference data"/>
+        <s v="StaffPersonal"/>
+        <s v="LEAInfo"/>
+        <s v="SchoolInfo"/>
+        <s v="StudentPersonal"/>
+        <s v="StudentSchoolEnrollment"/>
+        <s v="StaffAssignment"/>
+        <s v="StudentContactPersonal"/>
+        <s v="StudentContactRelationship"/>
+        <s v="Party, Identity, PersonPicture &amp; PrivacyObligation(s)"/>
+        <s v="LearningResourcePackage"/>
+        <s v="LearningResource"/>
+        <s v="EquipmentInfo"/>
+        <s v="RoomInfo"/>
+        <s v="ResourceList"/>
+        <s v="LibraryPatronStatus"/>
+        <s v="TermInfo"/>
+        <s v="SchoolCourseInfo"/>
+        <s v="SectionInfo"/>
+        <s v="StudentSectionEnrollment"/>
+        <s v="TimeTable"/>
+        <s v="TimeTableSubject"/>
+        <s v="TeachingGroup"/>
+        <s v="TimeTableCell"/>
+        <s v="TimeTableContainer"/>
+        <s v="ScheduledActivity"/>
+        <s v="ResourceBooking"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SelectStarQuery" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="FileName_SelectOnly" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="FileName_InsertData" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="265">
+  <r>
+    <n v="1"/>
+    <s v="Dim0StaffEmploymentStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StaffEmploymentStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="Dim0ElectronicIdType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ElectronicIdType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="Dim0NameUsageType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0NameUsageType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="Dim0YesNoType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0YesNoType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <s v="Dim0IndigenousStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0IndigenousStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <s v="Dim0SexCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SexCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <s v="Dim0BirthdateVerification"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0BirthdateVerification;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <s v="Dim0StateTerritoryCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StateTerritoryCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <s v="Dim0AustralianCitizenshipStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AustralianCitizenshipStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <s v="Dim0EnglishProficiency"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EnglishProficiency;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <s v="Dim0DwellingArrangement"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0DwellingArrangement;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <s v="Dim0ReligionType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ReligionType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <s v="Dim0PermanentResidentStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PermanentResidentStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <s v="Dim0VisaStudyEntitlement"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0VisaStudyEntitlement;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <s v="Dim0ImmunisationCertificateStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ImmunisationCertificateStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <s v="Dim0CulturalEthnicGroups"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0CulturalEthnicGroups;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <s v="Dim0MaritalStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0MaritalStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <s v="Dim0AddressType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AddressType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <s v="Dim0AddressRole"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AddressRole;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <s v="Dim0SpatialUnitType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SpatialUnitType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <s v="Dim0PhoneNumberType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PhoneNumberType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <s v="Dim0EmailType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EmailType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <s v="Dim0AlertMessageType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AlertMessageType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <s v="Dim0MedicalSeverity"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0MedicalSeverity;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <s v="Dim0DisabilityNCCDCategory"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0DisabilityNCCDCategory;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <s v="Dim0PrePrimaryEducationHours"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PrePrimaryEducationHours;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <s v="Dim0SchoolEnrollmentType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolEnrollmentType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <s v="Dim0FFPOSStatusCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0FFPOSStatusCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <s v="Dim0DisabilityLevelOfAdjustment"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0DisabilityLevelOfAdjustment;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <s v="Dim0BoardingStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0BoardingStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <s v="Dim0EmploymentType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EmploymentType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <s v="Dim0SchoolEducationLevelType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolEducationLevelType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <s v="Dim0NonSchoolEducationType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0NonSchoolEducationType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <s v="Dim0EducationAgencyType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EducationAgencyType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <s v="Dim0OperationalStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0OperationalStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <s v="Dim0SchoolLevelType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolLevelType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <s v="Dim0SchoolFocusCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolFocusCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <s v="Dim0ARIAClass"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ARIAClass;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <s v="Dim0SessionType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SessionType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <s v="Dim0YearLevelCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0YearLevelCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <s v="Dim0FederalElectorateList"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0FederalElectorateList;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <s v="Dim0SchoolSectorCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolSectorCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <s v="Dim0SystemicStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SystemicStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <s v="Dim0SchoolSystemType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolSystemType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <s v="Dim0SchoolGeographicLocationType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolGeographicLocationType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <s v="Dim0SchoolCoEdStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SchoolCoEdStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <s v="Dim0AusTimeZoneList"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AusTimeZoneList;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <s v="Dim0PartyType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PartyType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <s v="Dim0AuthenticationSource"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AuthenticationSource;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <s v="Dim0EncryptionAlgorithm"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EncryptionAlgorithm;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <s v="Dim0PermissionCategoryCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PermissionCategoryCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <s v="Dim0PermissionYesNoType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PermissionYesNoType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="53"/>
+    <s v="Dim0StaffActivity"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StaffActivity;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <s v="Dim0RelationshipToStudentType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0RelationshipToStudentType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="55"/>
+    <s v="Dim0ParentRelationshipStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ParentRelationshipStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="56"/>
+    <s v="Dim0ContactSourceType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ContactSourceType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <s v="Dim0ContactMethod"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ContactMethod;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <s v="Dim0CodesetForOtherCodeListType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0CodesetForOtherCodeListType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <s v="Dim0EnrollmentTimeFrame"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EnrollmentTimeFrame;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <s v="Dim0EnrollmentEntryType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EnrollmentEntryType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <s v="Dim0EnrollmentExitWithdrawalType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EnrollmentExitWithdrawalType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <s v="Dim0EnrollmentExitWithdrawalStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EnrollmentExitWithdrawalStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <s v="Dim0StudentSchoolEnrollmentOtherCodeField"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StudentSchoolEnrollmentOtherCodeField;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <s v="Dim0FullTimePartTimeStatusCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0FullTimePartTimeStatusCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <s v="Dim0PublicSchoolCatchmentStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0PublicSchoolCatchmentStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <s v="Dim0StudentSchoolEnrollmentRecordClosureReason"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StudentSchoolEnrollmentRecordClosureReason;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="67"/>
+    <s v="Dim0StudentSchoolEnrollmentPromotionStatus"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StudentSchoolEnrollmentPromotionStatus;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="68"/>
+    <s v="Dim0TravelMode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TravelMode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <s v="Dim0TravelAccompaniment"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TravelAccompaniment;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <s v="Dim0StudentGroupCategoryCode"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0StudentGroupCategoryCode;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <s v="Dim0AbstractContentType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AbstractContentType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <s v="Dim0AustralianCurriculumStrand"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AustralianCurriculumStrand;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <s v="Dim0TermInfoSessionType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TermInfoSessionType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <s v="Dim0EquipmentType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0EquipmentType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <s v="Dim0OwnerOrLocationSIF_RefObject"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0OwnerOrLocationSIF_RefObject;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <s v="Dim0ResourceType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ResourceType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <s v="Dim0YesNoOnly"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0YesNoOnly;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <s v="Dim0AcademicYearEntryType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0AcademicYearEntryType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <s v="Dim0TeacherCoverCredit"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TeacherCoverCredit;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <s v="Dim0TeacherCoverSupervision"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TeacherCoverSupervision;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <s v="Dim0ScheduledActivityType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ScheduledActivityType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <s v="Dim0TimeTableChangeType"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0TimeTableChangeType;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <s v="Dim0MediumOfInstruction"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0MediumOfInstruction;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <s v="Dim0LanguageOfInstruction"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0LanguageOfInstruction;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="85"/>
+    <s v="Dim0ReceivingLocationOfInstruction"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0ReceivingLocationOfInstruction;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <s v="Dim0SectionInfoOtherCodeField"/>
+    <s v="✅"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim0SectionInfoOtherCodeField;"/>
+    <s v="N/A"/>
+    <s v="Drop-then-Create-SIF-tables.sql"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <s v="Dim1Country"/>
+    <s v="✅"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1Country;"/>
+    <s v="001.001_Dim1Country_SelectOnly.sql"/>
+    <s v="001.001_Dim1Country_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <s v="Dim1Languages"/>
+    <s v="✅"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1Languages;"/>
+    <s v="001.002_Dim1Languages_SelectOnly.sql"/>
+    <s v="001.002_Dim1Languages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <s v="Dim1VisaSubClass"/>
+    <s v="✅"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1VisaSubClass;"/>
+    <s v="001.003_Dim1VisaSubClass_SelectOnly.sql"/>
+    <s v="001.003_Dim1VisaSubClass_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <s v="Dim1StaffPersonal"/>
+    <s v="✅"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StaffPersonal;"/>
+    <s v="002.001_Dim1StaffPersonal_SelectOnly.sql"/>
+    <s v="002.001_Dim1StaffPersonal_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <s v="Dim1StaffHouseholdContactInfo"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StaffHouseholdContactInfo;"/>
+    <s v="002.002_Dim1StaffHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="002.002_Dim1StaffHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <s v="Dim2StaffList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffList;"/>
+    <s v="002.003_Dim2StaffList_SelectOnly.sql"/>
+    <s v="002.003_Dim2StaffList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <s v="Dim2StaffElectronicIdList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffElectronicIdList;"/>
+    <s v="002.004_Dim2StaffElectronicIdList_SelectOnly.sql"/>
+    <s v="002.004_Dim2StaffElectronicIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <s v="Dim2StaffOtherIdList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffOtherIdList;"/>
+    <s v="002.005_Dim2StaffOtherIdList_SelectOnly.sql"/>
+    <s v="002.005_Dim2StaffOtherIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <s v="Dim2StaffNames"/>
+    <s v="✅"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffNames;"/>
+    <s v="002.006_Dim2StaffNames_SelectOnly.sql"/>
+    <s v="002.006_Dim2StaffNames_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <s v="Dim2StaffDemographics"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffDemographics;"/>
+    <s v="002.007_Dim2StaffDemographics_SelectOnly.sql"/>
+    <s v="002.007_Dim2StaffDemographics_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <s v="Bridge2StaffCountriesOfCitizenship"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StaffCountriesOfCitizenship;"/>
+    <s v="002.008_Bridge2StaffCountriesOfCitizenship_SelectOnly.sql"/>
+    <s v="002.008_Bridge2StaffCountriesOfCitizenship_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <s v="Bridge2StaffCountriesOfResidency"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StaffCountriesOfResidency;"/>
+    <s v="002.009_Bridge2StaffCountriesOfResidency_SelectOnly.sql"/>
+    <s v="002.009_Bridge2StaffCountriesOfResidency_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="107"/>
+    <s v="Bridge2StaffLanguages"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StaffLanguages;"/>
+    <s v="002.010_Bridge2StaffLanguages_SelectOnly.sql"/>
+    <s v="002.010_Bridge2StaffLanguages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="108"/>
+    <s v="Dim2StaffReligiousEvent"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffReligiousEvent;"/>
+    <s v="002.011_Dim2StaffReligiousEvent_SelectOnly.sql"/>
+    <s v="002.011_Dim2StaffReligiousEvent_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="109"/>
+    <s v="Dim2StaffPassport"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffPassport;"/>
+    <s v="002.012_Dim2StaffPassport_SelectOnly.sql"/>
+    <s v="002.012_Dim2StaffPassport_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="110"/>
+    <s v="Dim2StaffAddressList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffAddressList;"/>
+    <s v="002.013_Dim2StaffAddressList_SelectOnly.sql"/>
+    <s v="002.013_Dim2StaffAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="111"/>
+    <s v="Dim2StaffPhoneNumberList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffPhoneNumberList;"/>
+    <s v="002.014_Dim2StaffPhoneNumberList_SelectOnly.sql"/>
+    <s v="002.014_Dim2StaffPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="112"/>
+    <s v="Dim2StaffEmailList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffEmailList;"/>
+    <s v="002.015_Dim2StaffEmailList_SelectOnly.sql"/>
+    <s v="002.015_Dim2StaffEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="113"/>
+    <s v="Bridge2StaffHouseholdContactInfo"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StaffHouseholdContactInfo;"/>
+    <s v="002.016_Bridge2StaffHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="002.016_Bridge2StaffHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <s v="Dim2StaffHouseholdContactAddressList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffHouseholdContactAddressList;"/>
+    <s v="002.017_Dim2StaffHouseholdContactAddressList_SelectOnly.sql"/>
+    <s v="002.017_Dim2StaffHouseholdContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="115"/>
+    <s v="Dim2StaffHouseholdContactPhoneNumberList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffHouseholdContactPhoneNumberList;"/>
+    <s v="002.018_Dim2StaffHouseholdContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="002.018_Dim2StaffHouseholdContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="116"/>
+    <s v="Dim2StaffHouseholdContactEmailList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffHouseholdContactEmailList;"/>
+    <s v="002.019_Dim2StaffHouseholdContactEmailList_SelectOnly.sql"/>
+    <s v="002.019_Dim2StaffHouseholdContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="117"/>
+    <s v="Dim2StaffMostRecentNAPLANClassList"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StaffMostRecentNAPLANClassList;"/>
+    <s v="002.020_Dim2StaffMostRecentNAPLANClassList_SelectOnly.sql"/>
+    <s v="002.020_Dim2StaffMostRecentNAPLANClassList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="193"/>
+    <s v="Dim4StaffPersonalMostRecent"/>
+    <m/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4StaffPersonalMostRecent;"/>
+    <s v="002.021_Dim4StaffPersonalMostRecent_SelectOnly.sql"/>
+    <s v="002.021_Dim4StaffPersonalMostRecent_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <s v="Dim1LEAInfo"/>
+    <s v="✅"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1LEAInfo;"/>
+    <s v="003.001_Dim1LEAInfo_SelectOnly.sql"/>
+    <s v="003.001_Dim1LEAInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="153"/>
+    <s v="Dim2LEAAddressList"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2LEAAddressList;"/>
+    <s v="003.002_Dim2LEAAddressList_SelectOnly.sql"/>
+    <s v="003.002_Dim2LEAAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="154"/>
+    <s v="Dim2LEAPhoneNumberList"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2LEAPhoneNumberList;"/>
+    <s v="003.003_Dim2LEAPhoneNumberList_SelectOnly.sql"/>
+    <s v="003.003_Dim2LEAPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="155"/>
+    <s v="Dim2LEAContactInfo"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2LEAContactInfo;"/>
+    <s v="003.004_Dim2LEAContactInfo_SelectOnly.sql"/>
+    <s v="003.004_Dim2LEAContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="159"/>
+    <s v="Dim3LEAContactAddressList"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LEAContactAddressList;"/>
+    <s v="003.005_Dim3LEAContactAddressList_SelectOnly.sql"/>
+    <s v="003.005_Dim3LEAContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="160"/>
+    <s v="Dim3LEAContactPhoneNumberList"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LEAContactPhoneNumberList;"/>
+    <s v="003.006_Dim3LEAContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="003.006_Dim3LEAContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="161"/>
+    <s v="Dim3LEAContactEmailList"/>
+    <m/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LEAContactEmailList;"/>
+    <s v="003.007_Dim3LEAContactEmailList_SelectOnly.sql"/>
+    <s v="003.007_Dim3LEAContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="156"/>
+    <s v="Dim2SchoolInfo"/>
+    <s v="✅"/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2SchoolInfo;"/>
+    <s v="004.001_Dim2SchoolInfo_SelectOnly.sql"/>
+    <s v="004.001_Dim2SchoolInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="162"/>
+    <s v="Dim3SchoolACARAIdList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolACARAIdList;"/>
+    <s v="004.002_Dim3SchoolACARAIdList_SelectOnly.sql"/>
+    <s v="004.002_Dim3SchoolACARAIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="163"/>
+    <s v="Dim3SchoolOtherIdList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolOtherIdList;"/>
+    <s v="004.003_Dim3SchoolOtherIdList_SelectOnly.sql"/>
+    <s v="004.003_Dim3SchoolOtherIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="164"/>
+    <s v="Dim3SchoolFocus"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolFocus;"/>
+    <s v="004.004_Dim3SchoolFocus_SelectOnly.sql"/>
+    <s v="004.004_Dim3SchoolFocus_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="165"/>
+    <s v="Dim3SchoolAddressList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolAddressList;"/>
+    <s v="004.005_Dim3SchoolAddressList_SelectOnly.sql"/>
+    <s v="004.005_Dim3SchoolAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="166"/>
+    <s v="Dim3SchoolPhoneNumberList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolPhoneNumberList;"/>
+    <s v="004.006_Dim3SchoolPhoneNumberList_SelectOnly.sql"/>
+    <s v="004.006_Dim3SchoolPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="167"/>
+    <s v="Dim3SchoolEmailList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolEmailList;"/>
+    <s v="004.007_Dim3SchoolEmailList_SelectOnly.sql"/>
+    <s v="004.007_Dim3SchoolEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="168"/>
+    <s v="Dim3SchoolPrincipalPhoneNumberList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolPrincipalPhoneNumberList;"/>
+    <s v="004.008_Dim3SchoolPrincipalPhoneNumberList_SelectOnly.sql"/>
+    <s v="004.008_Dim3SchoolPrincipalPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="169"/>
+    <s v="Dim3SchoolPrincipalEmailList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolPrincipalEmailList;"/>
+    <s v="004.009_Dim3SchoolPrincipalEmailList_SelectOnly.sql"/>
+    <s v="004.009_Dim3SchoolPrincipalEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="170"/>
+    <s v="Dim3SchoolContactInfo"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolContactInfo;"/>
+    <s v="004.010_Dim3SchoolContactInfo_SelectOnly.sql"/>
+    <s v="004.010_Dim3SchoolContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="171"/>
+    <s v="Dim3SchoolCampus"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolCampus;"/>
+    <s v="004.011_Dim3SchoolCampus_SelectOnly.sql"/>
+    <s v="004.011_Dim3SchoolCampus_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="172"/>
+    <s v="Dim3SchoolGroup"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolGroup;"/>
+    <s v="004.012_Dim3SchoolGroup_SelectOnly.sql"/>
+    <s v="004.012_Dim3SchoolGroup_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="173"/>
+    <s v="Dim3SchoolYearLevels"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolYearLevels;"/>
+    <s v="004.013_Dim3SchoolYearLevels_SelectOnly.sql"/>
+    <s v="004.013_Dim3SchoolYearLevels_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="174"/>
+    <s v="Dim3SchoolEnrollmentByYearLevel"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3SchoolEnrollmentByYearLevel;"/>
+    <s v="004.014_Dim3SchoolEnrollmentByYearLevel_SelectOnly.sql"/>
+    <s v="004.014_Dim3SchoolEnrollmentByYearLevel_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="195"/>
+    <s v="Dim4SchoolContactAddressList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4SchoolContactAddressList;"/>
+    <s v="004.015_Dim4SchoolContactAddressList_SelectOnly.sql"/>
+    <s v="004.015_Dim4SchoolContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="196"/>
+    <s v="Dim4SchoolContactPhoneNumberList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4SchoolContactPhoneNumberList;"/>
+    <s v="004.016_Dim4SchoolContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="004.016_Dim4SchoolContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="197"/>
+    <s v="Dim4SchoolContactEmailList"/>
+    <m/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4SchoolContactEmailList;"/>
+    <s v="004.017_Dim4SchoolContactEmailList_SelectOnly.sql"/>
+    <s v="004.017_Dim4SchoolContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <s v="Dim1StudentPersonal"/>
+    <s v="✅"/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StudentPersonal;"/>
+    <s v="005.001_Dim1StudentPersonal_SelectOnly.sql"/>
+    <s v="005.001_Dim1StudentPersonal_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <s v="Dim1StudentHouseholdContactInfo"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StudentHouseholdContactInfo;"/>
+    <s v="005.002_Dim1StudentHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="005.002_Dim1StudentHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="118"/>
+    <s v="Dim2StudentList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentList;"/>
+    <s v="005.003_Dim2StudentList_SelectOnly.sql"/>
+    <s v="005.003_Dim2StudentList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="119"/>
+    <s v="Dim2StudentAlertMessages"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentAlertMessages;"/>
+    <s v="005.004_Dim2StudentAlertMessages_SelectOnly.sql"/>
+    <s v="005.004_Dim2StudentAlertMessages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="120"/>
+    <s v="Dim2StudentMedicalAlertMessages"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentMedicalAlertMessages;"/>
+    <s v="005.005_Dim2StudentMedicalAlertMessages_SelectOnly.sql"/>
+    <s v="005.005_Dim2StudentMedicalAlertMessages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="121"/>
+    <s v="Dim2StudentElectronicIdList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentElectronicIdList;"/>
+    <s v="005.006_Dim2StudentElectronicIdList_SelectOnly.sql"/>
+    <s v="005.006_Dim2StudentElectronicIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="122"/>
+    <s v="Dim2StudentOtherIdList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentOtherIdList;"/>
+    <s v="005.007_Dim2StudentOtherIdList_SelectOnly.sql"/>
+    <s v="005.007_Dim2StudentOtherIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="123"/>
+    <s v="Dim2StudentNames"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentNames;"/>
+    <s v="005.008_Dim2StudentNames_SelectOnly.sql"/>
+    <s v="005.008_Dim2StudentNames_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="124"/>
+    <s v="Dim2StudentDemographics"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentDemographics;"/>
+    <s v="005.009_Dim2StudentDemographics_SelectOnly.sql"/>
+    <s v="005.009_Dim2StudentDemographics_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="125"/>
+    <s v="Bridge2StudentCountriesOfCitizenship"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentCountriesOfCitizenship;"/>
+    <s v="005.010_Bridge2StudentCountriesOfCitizenship_SelectOnly.sql"/>
+    <s v="005.010_Bridge2StudentCountriesOfCitizenship_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="126"/>
+    <s v="Bridge2StudentCountriesOfResidency"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentCountriesOfResidency;"/>
+    <s v="005.011_Bridge2StudentCountriesOfResidency_SelectOnly.sql"/>
+    <s v="005.011_Bridge2StudentCountriesOfResidency_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="127"/>
+    <s v="Bridge2StudentLanguages"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentLanguages;"/>
+    <s v="005.012_Bridge2StudentLanguages_SelectOnly.sql"/>
+    <s v="005.012_Bridge2StudentLanguages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="128"/>
+    <s v="Dim2StudentReligiousEvent"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentReligiousEvent;"/>
+    <s v="005.013_Dim2StudentReligiousEvent_SelectOnly.sql"/>
+    <s v="005.013_Dim2StudentReligiousEvent_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="129"/>
+    <s v="Dim2StudentPassport"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentPassport;"/>
+    <s v="005.014_Dim2StudentPassport_SelectOnly.sql"/>
+    <s v="005.014_Dim2StudentPassport_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="130"/>
+    <s v="Dim2StudentAddressList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentAddressList;"/>
+    <s v="005.015_Dim2StudentAddressList_SelectOnly.sql"/>
+    <s v="005.015_Dim2StudentAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="131"/>
+    <s v="Dim2StudentPhoneNumberList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentPhoneNumberList;"/>
+    <s v="005.016_Dim2StudentPhoneNumberList_SelectOnly.sql"/>
+    <s v="005.016_Dim2StudentPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="132"/>
+    <s v="Dim2StudentEmailList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentEmailList;"/>
+    <s v="005.017_Dim2StudentEmailList_SelectOnly.sql"/>
+    <s v="005.017_Dim2StudentEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="133"/>
+    <s v="Bridge2StudentHouseholdContactInfo"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentHouseholdContactInfo;"/>
+    <s v="005.018_Bridge2StudentHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="005.018_Bridge2StudentHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="134"/>
+    <s v="Dim2StudentHouseholdContactAddressList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentHouseholdContactAddressList;"/>
+    <s v="005.019_Dim2StudentHouseholdContactAddressList_SelectOnly.sql"/>
+    <s v="005.019_Dim2StudentHouseholdContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="135"/>
+    <s v="Dim2StudentHouseholdContactPhoneNumberList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentHouseholdContactPhoneNumberList;"/>
+    <s v="005.020_Dim2StudentHouseholdContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="005.020_Dim2StudentHouseholdContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="136"/>
+    <s v="Dim2StudentHouseholdContactEmailList"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentHouseholdContactEmailList;"/>
+    <s v="005.021_Dim2StudentHouseholdContactEmailList_SelectOnly.sql"/>
+    <s v="005.021_Dim2StudentHouseholdContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="194"/>
+    <s v="Dim4StudentPersonalMostRecent"/>
+    <m/>
+    <x v="5"/>
+    <x v="5"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4StudentPersonalMostRecent;"/>
+    <s v="005.022_Dim4StudentPersonalMostRecent_SelectOnly.sql"/>
+    <s v="005.022_Dim4StudentPersonalMostRecent_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="180"/>
+    <s v="Fact3StudentSchoolEnrollment"/>
+    <s v="✅"/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact3StudentSchoolEnrollment;"/>
+    <s v="006.001_Fact3StudentSchoolEnrollment_SelectOnly.sql"/>
+    <s v="006.001_Fact3StudentSchoolEnrollment_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="210"/>
+    <s v="Fact4StudentSchoolEnrollmentOtherCodes"/>
+    <m/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StudentSchoolEnrollmentOtherCodes;"/>
+    <s v="006.002_Fact4StudentSchoolEnrollmentOtherCodes_SelectOnly.sql"/>
+    <s v="006.002_Fact4StudentSchoolEnrollmentOtherCodes_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="211"/>
+    <s v="Fact4StudentSchoolEnrollmentStudentGroup"/>
+    <m/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StudentSchoolEnrollmentStudentGroup;"/>
+    <s v="006.003_Fact4StudentSchoolEnrollmentStudentGroup_SelectOnly.sql"/>
+    <s v="006.003_Fact4StudentSchoolEnrollmentStudentGroup_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="212"/>
+    <s v="Fact4StudentSchoolEnrollmentPublishingPermissions"/>
+    <m/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StudentSchoolEnrollmentPublishingPermissions;"/>
+    <s v="006.004_Fact4StudentSchoolEnrollmentPublishingPermissions_SelectOnly.sql"/>
+    <s v="006.004_Fact4StudentSchoolEnrollmentPublishingPermissions_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="237"/>
+    <s v="Fact6StudentSubjectChoice"/>
+    <m/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact6StudentSubjectChoice;"/>
+    <s v="006.005_Fact6StudentSubjectChoice_SelectOnly.sql"/>
+    <s v="006.005_Fact6StudentSubjectChoice_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="238"/>
+    <s v="Fact6StudentSubjectChoiceOtherCode"/>
+    <m/>
+    <x v="6"/>
+    <x v="6"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact6StudentSubjectChoiceOtherCode;"/>
+    <s v="006.006_Fact6StudentSubjectChoiceOtherCode_SelectOnly.sql"/>
+    <s v="006.006_Fact6StudentSubjectChoiceOtherCode_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="178"/>
+    <s v="Fact3StaffAssignment"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact3StaffAssignment;"/>
+    <s v="007.001_Fact3StaffAssignment_SelectOnly.sql"/>
+    <s v="007.001_Fact3StaffAssignment_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="205"/>
+    <s v="Fact4StaffAssignmentActivityExtension"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StaffAssignmentActivityExtension;"/>
+    <s v="007.002_Fact4StaffAssignmentActivityExtension_SelectOnly.sql"/>
+    <s v="007.002_Fact4StaffAssignmentActivityExtension_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="206"/>
+    <s v="Fact4StaffAssignmentActivityExtensionOtherCode"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StaffAssignmentActivityExtensionOtherCode;"/>
+    <s v="007.003_Fact4StaffAssignmentActivityExtensionOtherCode_SelectOnly.sql"/>
+    <s v="007.003_Fact4StaffAssignmentActivityExtensionOtherCode_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="207"/>
+    <s v="Fact4StaffAssignmentYearLevels"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StaffAssignmentYearLevels;"/>
+    <s v="007.004_Fact4StaffAssignmentYearLevels_SelectOnly.sql"/>
+    <s v="007.004_Fact4StaffAssignmentYearLevels_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="208"/>
+    <s v="Fact4StaffAssignmentCalendarSummaryList"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StaffAssignmentCalendarSummaryList;"/>
+    <s v="007.005_Fact4StaffAssignmentCalendarSummaryList_SelectOnly.sql"/>
+    <s v="007.005_Fact4StaffAssignmentCalendarSummaryList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="236"/>
+    <s v="Fact6StaffAssignmentSubjectList"/>
+    <m/>
+    <x v="7"/>
+    <x v="7"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact6StaffAssignmentSubjectList;"/>
+    <s v="007.006_Fact6StaffAssignmentSubjectList_SelectOnly.sql"/>
+    <s v="007.006_Fact6StaffAssignmentSubjectList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <s v="Dim1StudentContactPersonal"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StudentContactPersonal;"/>
+    <s v="008.001_Dim1StudentContactPersonal_SelectOnly.sql"/>
+    <s v="008.001_Dim1StudentContactPersonal_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <s v="Dim1StudentContactHouseholdContactInfo"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1StudentContactHouseholdContactInfo;"/>
+    <s v="008.002_Dim1StudentContactHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="008.002_Dim1StudentContactHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="137"/>
+    <s v="Dim2StudentContactPersonList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactPersonList;"/>
+    <s v="008.003_Dim2StudentContactPersonList_SelectOnly.sql"/>
+    <s v="008.003_Dim2StudentContactPersonList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="138"/>
+    <s v="Dim2StudentContactOtherIdList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactOtherIdList;"/>
+    <s v="008.004_Dim2StudentContactOtherIdList_SelectOnly.sql"/>
+    <s v="008.004_Dim2StudentContactOtherIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="139"/>
+    <s v="Dim2StudentContactNames"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactNames;"/>
+    <s v="008.005_Dim2StudentContactNames_SelectOnly.sql"/>
+    <s v="008.005_Dim2StudentContactNames_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="140"/>
+    <s v="Dim2StudentContactDemographics"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactDemographics;"/>
+    <s v="008.006_Dim2StudentContactDemographics_SelectOnly.sql"/>
+    <s v="008.006_Dim2StudentContactDemographics_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="141"/>
+    <s v="Bridge2StudentContactCountriesOfCitizenship"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentContactCountriesOfCitizenship;"/>
+    <s v="008.007_Bridge2StudentContactCountriesOfCitizenship_SelectOnly.sql"/>
+    <s v="008.007_Bridge2StudentContactCountriesOfCitizenship_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="142"/>
+    <s v="Bridge2StudentContactCountriesOfResidency"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentContactCountriesOfResidency;"/>
+    <s v="008.008_Bridge2StudentContactCountriesOfResidency_SelectOnly.sql"/>
+    <s v="008.008_Bridge2StudentContactCountriesOfResidency_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="143"/>
+    <s v="Bridge2StudentContactLanguages"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentContactLanguages;"/>
+    <s v="008.009_Bridge2StudentContactLanguages_SelectOnly.sql"/>
+    <s v="008.009_Bridge2StudentContactLanguages_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="144"/>
+    <s v="Dim2StudentContactReligiousEvent"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactReligiousEvent;"/>
+    <s v="008.010_Dim2StudentContactReligiousEvent_SelectOnly.sql"/>
+    <s v="008.010_Dim2StudentContactReligiousEvent_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="145"/>
+    <s v="Dim2StudentContactPassport"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactPassport;"/>
+    <s v="008.011_Dim2StudentContactPassport_SelectOnly.sql"/>
+    <s v="008.011_Dim2StudentContactPassport_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="146"/>
+    <s v="Dim2StudentContactAddressList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactAddressList;"/>
+    <s v="008.012_Dim2StudentContactAddressList_SelectOnly.sql"/>
+    <s v="008.012_Dim2StudentContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="147"/>
+    <s v="Dim2StudentContactPhoneNumberList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactPhoneNumberList;"/>
+    <s v="008.013_Dim2StudentContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="008.013_Dim2StudentContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="148"/>
+    <s v="Dim2StudentContactEmailList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactEmailList;"/>
+    <s v="008.014_Dim2StudentContactEmailList_SelectOnly.sql"/>
+    <s v="008.014_Dim2StudentContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="149"/>
+    <s v="Bridge2StudentContactHouseholdContactInfo"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Bridge2StudentContactHouseholdContactInfo;"/>
+    <s v="008.015_Bridge2StudentContactHouseholdContactInfo_SelectOnly.sql"/>
+    <s v="008.015_Bridge2StudentContactHouseholdContactInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="150"/>
+    <s v="Dim2StudentContactHouseholdContactAddressList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactHouseholdContactAddressList;"/>
+    <s v="008.016_Dim2StudentContactHouseholdContactAddressList_SelectOnly.sql"/>
+    <s v="008.016_Dim2StudentContactHouseholdContactAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="151"/>
+    <s v="Dim2StudentContactHouseholdContactPhoneNumberList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactHouseholdContactPhoneNumberList;"/>
+    <s v="008.017_Dim2StudentContactHouseholdContactPhoneNumberList_SelectOnly.sql"/>
+    <s v="008.017_Dim2StudentContactHouseholdContactPhoneNumberList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="152"/>
+    <s v="Dim2StudentContactHouseholdContactEmailList"/>
+    <m/>
+    <x v="8"/>
+    <x v="8"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2StudentContactHouseholdContactEmailList;"/>
+    <s v="008.018_Dim2StudentContactHouseholdContactEmailList_SelectOnly.sql"/>
+    <s v="008.018_Dim2StudentContactHouseholdContactEmailList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="179"/>
+    <s v="Fact3StudentContactRelationship"/>
+    <m/>
+    <x v="9"/>
+    <x v="9"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact3StudentContactRelationship;"/>
+    <s v="009.001_Fact3StudentContactRelationship_SelectOnly.sql"/>
+    <s v="009.001_Fact3StudentContactRelationship_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="209"/>
+    <s v="Fact4StudentContactRelationshipHouseholdList"/>
+    <m/>
+    <x v="9"/>
+    <x v="9"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact4StudentContactRelationshipHouseholdList;"/>
+    <s v="009.002_Fact4StudentContactRelationshipHouseholdList_SelectOnly.sql"/>
+    <s v="009.002_Fact4StudentContactRelationshipHouseholdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="157"/>
+    <s v="Dim2PartyList"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2PartyList;"/>
+    <s v="010.001_Dim2PartyList_SelectOnly.sql"/>
+    <s v="010.001_Dim2PartyList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="175"/>
+    <s v="Dim3Identity"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3Identity;"/>
+    <s v="010.002_Dim3Identity_SelectOnly.sql"/>
+    <s v="010.002_Dim3Identity_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="176"/>
+    <s v="Dim3PersonPicture"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3PersonPicture;"/>
+    <s v="010.003_Dim3PersonPicture_SelectOnly.sql"/>
+    <s v="010.003_Dim3PersonPicture_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="177"/>
+    <s v="Dim3PersonPrivacyObligationDocument"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3PersonPrivacyObligationDocument;"/>
+    <s v="010.004_Dim3PersonPrivacyObligationDocument_SelectOnly.sql"/>
+    <s v="010.004_Dim3PersonPrivacyObligationDocument_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="198"/>
+    <s v="Dim4IdentityAssertions"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4IdentityAssertions;"/>
+    <s v="010.005_Dim4IdentityAssertions_SelectOnly.sql"/>
+    <s v="010.005_Dim4IdentityAssertions_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="199"/>
+    <s v="Dim4IdentityPasswordList"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4IdentityPasswordList;"/>
+    <s v="010.006_Dim4IdentityPasswordList_SelectOnly.sql"/>
+    <s v="010.006_Dim4IdentityPasswordList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="200"/>
+    <s v="Dim4PersonPicturePublishingPermissions"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4PersonPicturePublishingPermissions;"/>
+    <s v="010.007_Dim4PersonPicturePublishingPermissions_SelectOnly.sql"/>
+    <s v="010.007_Dim4PersonPicturePublishingPermissions_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="201"/>
+    <s v="Dim4PersonPrivacySettingLocation"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4PersonPrivacySettingLocation;"/>
+    <s v="010.008_Dim4PersonPrivacySettingLocation_SelectOnly.sql"/>
+    <s v="010.008_Dim4PersonPrivacySettingLocation_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="202"/>
+    <s v="Dim4PersonPrivacyDataDomain"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4PersonPrivacyDataDomain;"/>
+    <s v="010.009_Dim4PersonPrivacyDataDomain_SelectOnly.sql"/>
+    <s v="010.009_Dim4PersonPrivacyDataDomain_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="203"/>
+    <s v="Dim4PersonPrivacyPermissionToParticipate"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4PersonPrivacyPermissionToParticipate;"/>
+    <s v="010.010_Dim4PersonPrivacyPermissionToParticipate_SelectOnly.sql"/>
+    <s v="010.010_Dim4PersonPrivacyPermissionToParticipate_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="204"/>
+    <s v="Dim4PersonPrivacyApplicableLaw"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4PersonPrivacyApplicableLaw;"/>
+    <s v="010.011_Dim4PersonPrivacyApplicableLaw_SelectOnly.sql"/>
+    <s v="010.011_Dim4PersonPrivacyApplicableLaw_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="228"/>
+    <s v="Dim5PersonPrivacyDataDomainShareWith"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5PersonPrivacyDataDomainShareWith;"/>
+    <s v="010.012_Dim5PersonPrivacyDataDomainShareWith_SelectOnly.sql"/>
+    <s v="010.012_Dim5PersonPrivacyDataDomainShareWith_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="229"/>
+    <s v="Dim5PersonPrivacyDataDomainDoNotShareWith"/>
+    <m/>
+    <x v="10"/>
+    <x v="10"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5PersonPrivacyDataDomainDoNotShareWith;"/>
+    <s v="010.013_Dim5PersonPrivacyDataDomainDoNotShareWith_SelectOnly.sql"/>
+    <s v="010.013_Dim5PersonPrivacyDataDomainDoNotShareWith_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <s v="Dim1LearningResourcePackage"/>
+    <m/>
+    <x v="11"/>
+    <x v="11"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1LearningResourcePackage;"/>
+    <s v="011.001_Dim1LearningResourcePackage_SelectOnly.sql"/>
+    <s v="011.001_Dim1LearningResourcePackage_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="158"/>
+    <s v="Dim2LearningResource"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim2LearningResource;"/>
+    <s v="012.001_Dim2LearningResource_SelectOnly.sql"/>
+    <s v="012.001_Dim2LearningResource_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="181"/>
+    <s v="Dim3LearningResourceContacts"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceContacts;"/>
+    <s v="012.002_Dim3LearningResourceContacts_SelectOnly.sql"/>
+    <s v="012.002_Dim3LearningResourceContacts_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="182"/>
+    <s v="Dim3LearningResourceYearLevels"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceYearLevels;"/>
+    <s v="012.003_Dim3LearningResourceYearLevels_SelectOnly.sql"/>
+    <s v="012.003_Dim3LearningResourceYearLevels_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="183"/>
+    <s v="Dim3LearningResourceAustralianCurriculumStrandList"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceAustralianCurriculumStrandList;"/>
+    <s v="012.004_Dim3LearningResourceAustralianCurriculumStrandList_SelectOnly.sql"/>
+    <s v="012.004_Dim3LearningResourceAustralianCurriculumStrandList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="184"/>
+    <s v="Dim3LearningResourceSubjectAreaList"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceSubjectAreaList;"/>
+    <s v="012.005_Dim3LearningResourceSubjectAreaList_SelectOnly.sql"/>
+    <s v="012.005_Dim3LearningResourceSubjectAreaList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="185"/>
+    <s v="Dim3LearningResourceMediaTypes"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceMediaTypes;"/>
+    <s v="012.006_Dim3LearningResourceMediaTypes_SelectOnly.sql"/>
+    <s v="012.006_Dim3LearningResourceMediaTypes_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="186"/>
+    <s v="Dim3LearningResourceApprovals"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceApprovals;"/>
+    <s v="012.007_Dim3LearningResourceApprovals_SelectOnly.sql"/>
+    <s v="012.007_Dim3LearningResourceApprovals_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="187"/>
+    <s v="Dim3LearningResourceEvaluations"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceEvaluations;"/>
+    <s v="012.008_Dim3LearningResourceEvaluations_SelectOnly.sql"/>
+    <s v="012.008_Dim3LearningResourceEvaluations_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="188"/>
+    <s v="Dim3LearningResourceComponents"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LearningResourceComponents;"/>
+    <s v="012.009_Dim3LearningResourceComponents_SelectOnly.sql"/>
+    <s v="012.009_Dim3LearningResourceComponents_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="213"/>
+    <s v="Dim4LearningResourceContactNames"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceContactNames;"/>
+    <s v="012.010_Dim4LearningResourceContactNames_SelectOnly.sql"/>
+    <s v="012.010_Dim4LearningResourceContactNames_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="214"/>
+    <s v="Dim4LearningResourceContactAddresses"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceContactAddresses;"/>
+    <s v="012.011_Dim4LearningResourceContactAddresses_SelectOnly.sql"/>
+    <s v="012.011_Dim4LearningResourceContactAddresses_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="215"/>
+    <s v="Dim4LearningResourceContactPhoneNumbers"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceContactPhoneNumbers;"/>
+    <s v="012.012_Dim4LearningResourceContactPhoneNumbers_SelectOnly.sql"/>
+    <s v="012.012_Dim4LearningResourceContactPhoneNumbers_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="216"/>
+    <s v="Dim4LearningResourceContactEmails"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceContactEmails;"/>
+    <s v="012.013_Dim4LearningResourceContactEmails_SelectOnly.sql"/>
+    <s v="012.013_Dim4LearningResourceContactEmails_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="217"/>
+    <s v="Dim4LearningResourceSubjectAreaOtherCodeList"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceSubjectAreaOtherCodeList;"/>
+    <s v="012.014_Dim4LearningResourceSubjectAreaOtherCodeList_SelectOnly.sql"/>
+    <s v="012.014_Dim4LearningResourceSubjectAreaOtherCodeList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="218"/>
+    <s v="Dim4LearningResourceComponentTeachingLearningStrategies"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceComponentTeachingLearningStrategies;"/>
+    <s v="012.015_Dim4LearningResourceComponentTeachingLearningStrategies_SelectOnly.sql"/>
+    <s v="012.015_Dim4LearningResourceComponentTeachingLearningStrategies_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="219"/>
+    <s v="Dim4LearningResourceComponentAssociatedObjects"/>
+    <m/>
+    <x v="12"/>
+    <x v="12"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LearningResourceComponentAssociatedObjects;"/>
+    <s v="012.016_Dim4LearningResourceComponentAssociatedObjects_SelectOnly.sql"/>
+    <s v="012.016_Dim4LearningResourceComponentAssociatedObjects_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <s v="Dim1EquipmentInfo"/>
+    <m/>
+    <x v="13"/>
+    <x v="13"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1EquipmentInfo;"/>
+    <s v="013.001_Dim1EquipmentInfo_SelectOnly.sql"/>
+    <s v="013.001_Dim1EquipmentInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="191"/>
+    <s v="Dim3RoomInfo"/>
+    <m/>
+    <x v="14"/>
+    <x v="14"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3RoomInfo;"/>
+    <s v="014.001_Dim3RoomInfo_SelectOnly.sql"/>
+    <s v="014.001_Dim3RoomInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="223"/>
+    <s v="Dim4RoomInfoStaffList"/>
+    <m/>
+    <x v="14"/>
+    <x v="14"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4RoomInfoStaffList;"/>
+    <s v="014.002_Dim4RoomInfoStaffList_SelectOnly.sql"/>
+    <s v="014.002_Dim4RoomInfoStaffList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="224"/>
+    <s v="Dim4ResourceList"/>
+    <m/>
+    <x v="15"/>
+    <x v="15"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4ResourceList;"/>
+    <s v="015.001_Dim4ResourceList_SelectOnly.sql"/>
+    <s v="015.001_Dim4ResourceList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="190"/>
+    <s v="Dim3LibraryPatronStatus"/>
+    <m/>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3LibraryPatronStatus;"/>
+    <s v="016.001_Dim3LibraryPatronStatus_SelectOnly.sql"/>
+    <s v="016.001_Dim3LibraryPatronStatus_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="220"/>
+    <s v="Dim4LibraryPatronElectronicIdList"/>
+    <m/>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LibraryPatronElectronicIdList;"/>
+    <s v="016.002_Dim4LibraryPatronElectronicIdList_SelectOnly.sql"/>
+    <s v="016.002_Dim4LibraryPatronElectronicIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="221"/>
+    <s v="Dim4LibraryPatronTransactionList"/>
+    <m/>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LibraryPatronTransactionList;"/>
+    <s v="016.003_Dim4LibraryPatronTransactionList_SelectOnly.sql"/>
+    <s v="016.003_Dim4LibraryPatronTransactionList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="222"/>
+    <s v="Dim4LibraryPatronMessageList"/>
+    <m/>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4LibraryPatronMessageList;"/>
+    <s v="016.004_Dim4LibraryPatronMessageList_SelectOnly.sql"/>
+    <s v="016.004_Dim4LibraryPatronMessageList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="230"/>
+    <s v="Dim5LibraryItemElectronicIdList"/>
+    <m/>
+    <x v="16"/>
+    <x v="16"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5LibraryItemElectronicIdList;"/>
+    <s v="016.005_Dim5LibraryItemElectronicIdList_SelectOnly.sql"/>
+    <s v="016.005_Dim5LibraryItemElectronicIdList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="189"/>
+    <s v="Dim3TermInfo"/>
+    <m/>
+    <x v="17"/>
+    <x v="17"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3TermInfo;"/>
+    <s v="017.001_Dim3TermInfo_SelectOnly.sql"/>
+    <s v="017.001_Dim3TermInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="226"/>
+    <s v="Dim4SchoolCourseInfo"/>
+    <m/>
+    <x v="18"/>
+    <x v="18"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4SchoolCourseInfo;"/>
+    <s v="018.001_Dim4SchoolCourseInfo_SelectOnly.sql"/>
+    <s v="018.001_Dim4SchoolCourseInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="232"/>
+    <s v="Dim5SchoolCourseSubjectAreaList"/>
+    <m/>
+    <x v="18"/>
+    <x v="18"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5SchoolCourseSubjectAreaList;"/>
+    <s v="018.002_Dim5SchoolCourseSubjectAreaList_SelectOnly.sql"/>
+    <s v="018.002_Dim5SchoolCourseSubjectAreaList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="239"/>
+    <s v="Dim6SchoolCourseSubjectAreaOtherCodes"/>
+    <m/>
+    <x v="18"/>
+    <x v="18"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim6SchoolCourseSubjectAreaOtherCodes;"/>
+    <s v="018.003_Dim6SchoolCourseSubjectAreaOtherCodes_SelectOnly.sql"/>
+    <s v="018.003_Dim6SchoolCourseSubjectAreaOtherCodes_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="235"/>
+    <s v="Dim5SectionInfo"/>
+    <m/>
+    <x v="19"/>
+    <x v="19"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5SectionInfo;"/>
+    <s v="019.001_Dim5SectionInfo_SelectOnly.sql"/>
+    <s v="019.001_Dim5SectionInfo_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="242"/>
+    <s v="Dim6SectionInfoOtherCodes"/>
+    <m/>
+    <x v="19"/>
+    <x v="19"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim6SectionInfoOtherCodes;"/>
+    <s v="019.002_Dim6SectionInfoOtherCodes_SelectOnly.sql"/>
+    <s v="019.002_Dim6SectionInfoOtherCodes_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="243"/>
+    <s v="Fact6StudentSectionEnrollment"/>
+    <m/>
+    <x v="20"/>
+    <x v="20"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact6StudentSectionEnrollment;"/>
+    <s v="020.001_Fact6StudentSectionEnrollment_SelectOnly.sql"/>
+    <s v="020.001_Fact6StudentSectionEnrollment_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="192"/>
+    <s v="Dim3TimeTable"/>
+    <m/>
+    <x v="21"/>
+    <x v="21"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim3TimeTable;"/>
+    <s v="021.001_Dim3TimeTable_SelectOnly.sql"/>
+    <s v="021.001_Dim3TimeTable_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="225"/>
+    <s v="Dim4TimeTableDay"/>
+    <m/>
+    <x v="21"/>
+    <x v="21"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4TimeTableDay;"/>
+    <s v="021.002_Dim4TimeTableDay_SelectOnly.sql"/>
+    <s v="021.002_Dim4TimeTableDay_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="231"/>
+    <s v="Dim5TimeTablePeriod"/>
+    <m/>
+    <x v="21"/>
+    <x v="21"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5TimeTablePeriod;"/>
+    <s v="021.003_Dim5TimeTablePeriod_SelectOnly.sql"/>
+    <s v="021.003_Dim5TimeTablePeriod_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="233"/>
+    <s v="Dim5TimeTableSubject"/>
+    <m/>
+    <x v="22"/>
+    <x v="22"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5TimeTableSubject;"/>
+    <s v="022.001_Dim5TimeTableSubject_SelectOnly.sql"/>
+    <s v="022.001_Dim5TimeTableSubject_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="240"/>
+    <s v="Dim6TimeTableSubjectOtherCodes"/>
+    <m/>
+    <x v="22"/>
+    <x v="22"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim6TimeTableSubjectOtherCodes;"/>
+    <s v="022.002_Dim6TimeTableSubjectOtherCodes_SelectOnly.sql"/>
+    <s v="022.002_Dim6TimeTableSubjectOtherCodes_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="241"/>
+    <s v="Dim6TeachingGroup"/>
+    <m/>
+    <x v="23"/>
+    <x v="23"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim6TeachingGroup;"/>
+    <s v="023.001_Dim6TeachingGroup_SelectOnly.sql"/>
+    <s v="023.001_Dim6TeachingGroup_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="244"/>
+    <s v="Dim7TeachingGroupStudentList"/>
+    <m/>
+    <x v="23"/>
+    <x v="23"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim7TeachingGroupStudentList;"/>
+    <s v="023.002_Dim7TeachingGroupStudentList_SelectOnly.sql"/>
+    <s v="023.002_Dim7TeachingGroupStudentList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="245"/>
+    <s v="Dim7TeachingGroupTeacherList"/>
+    <m/>
+    <x v="23"/>
+    <x v="23"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim7TeachingGroupTeacherList;"/>
+    <s v="023.003_Dim7TeachingGroupTeacherList_SelectOnly.sql"/>
+    <s v="023.003_Dim7TeachingGroupTeacherList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="248"/>
+    <s v="Dim8TeachingGroupPeriodList"/>
+    <m/>
+    <x v="23"/>
+    <x v="23"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TeachingGroupPeriodList;"/>
+    <s v="023.004_Dim8TeachingGroupPeriodList_SelectOnly.sql"/>
+    <s v="023.004_Dim8TeachingGroupPeriodList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="246"/>
+    <s v="Dim7TimeTableCell"/>
+    <m/>
+    <x v="24"/>
+    <x v="24"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim7TimeTableCell;"/>
+    <s v="024.001_Dim7TimeTableCell_SelectOnly.sql"/>
+    <s v="024.001_Dim7TimeTableCell_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="249"/>
+    <s v="Dim8TimeTableCellTeacherCoverList"/>
+    <m/>
+    <x v="24"/>
+    <x v="24"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableCellTeacherCoverList;"/>
+    <s v="024.002_Dim8TimeTableCellTeacherCoverList_SelectOnly.sql"/>
+    <s v="024.002_Dim8TimeTableCellTeacherCoverList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="250"/>
+    <s v="Dim8TimeTableCellRoomList"/>
+    <m/>
+    <x v="24"/>
+    <x v="24"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableCellRoomList;"/>
+    <s v="024.003_Dim8TimeTableCellRoomList_SelectOnly.sql"/>
+    <s v="024.003_Dim8TimeTableCellRoomList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <s v="Dim1TimeTableContainer"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim1TimeTableContainer;"/>
+    <s v="025.001_Dim1TimeTableContainer_SelectOnly.sql"/>
+    <s v="025.001_Dim1TimeTableContainer_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="227"/>
+    <s v="Dim4TimeTableContainerSchedule"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim4TimeTableContainerSchedule;"/>
+    <s v="025.002_Dim4TimeTableContainerSchedule_SelectOnly.sql"/>
+    <s v="025.002_Dim4TimeTableContainerSchedule_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="234"/>
+    <s v="Dim5TimeTableContainerDay"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim5TimeTableContainerDay;"/>
+    <s v="025.003_Dim5TimeTableContainerDay_SelectOnly.sql"/>
+    <s v="025.003_Dim5TimeTableContainerDay_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="247"/>
+    <s v="Dim7TimeTableContainerTeachingGroupScheduleList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim7TimeTableContainerTeachingGroupScheduleList;"/>
+    <s v="025.004_Dim7TimeTableContainerTeachingGroupScheduleList_SelectOnly.sql"/>
+    <s v="025.004_Dim7TimeTableContainerTeachingGroupScheduleList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="251"/>
+    <s v="Dim8TimeTableContainerScheduleCellList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableContainerScheduleCellList;"/>
+    <s v="025.005_Dim8TimeTableContainerScheduleCellList_SelectOnly.sql"/>
+    <s v="025.005_Dim8TimeTableContainerScheduleCellList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="252"/>
+    <s v="Dim8TimeTableContainerTeachingGroupPeriodList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableContainerTeachingGroupPeriodList;"/>
+    <s v="025.006_Dim8TimeTableContainerTeachingGroupPeriodList_SelectOnly.sql"/>
+    <s v="025.006_Dim8TimeTableContainerTeachingGroupPeriodList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="253"/>
+    <s v="Dim8TimeTableContainerTeachingGroupStudentList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableContainerTeachingGroupStudentList;"/>
+    <s v="025.007_Dim8TimeTableContainerTeachingGroupStudentList_SelectOnly.sql"/>
+    <s v="025.007_Dim8TimeTableContainerTeachingGroupStudentList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="254"/>
+    <s v="Dim8TimeTableContainerTeachingGroupTeacherList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8TimeTableContainerTeachingGroupTeacherList;"/>
+    <s v="025.008_Dim8TimeTableContainerTeachingGroupTeacherList_SelectOnly.sql"/>
+    <s v="025.008_Dim8TimeTableContainerTeachingGroupTeacherList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="256"/>
+    <s v="Dim9TimeTableContainerTeacherCoverList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9TimeTableContainerTeacherCoverList;"/>
+    <s v="025.009_Dim9TimeTableContainerTeacherCoverList_SelectOnly.sql"/>
+    <s v="025.009_Dim9TimeTableContainerTeacherCoverList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="257"/>
+    <s v="Dim9TimeTableContainerRoomList"/>
+    <m/>
+    <x v="25"/>
+    <x v="25"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9TimeTableContainerRoomList;"/>
+    <s v="025.010_Dim9TimeTableContainerRoomList_SelectOnly.sql"/>
+    <s v="025.010_Dim9TimeTableContainerRoomList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="255"/>
+    <s v="Dim8ScheduledActivity"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim8ScheduledActivity;"/>
+    <s v="026.001_Dim8ScheduledActivity_SelectOnly.sql"/>
+    <s v="026.001_Dim8ScheduledActivity_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="258"/>
+    <s v="Dim9ScheduledActivityTeacherCoverList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityTeacherCoverList;"/>
+    <s v="026.002_Dim9ScheduledActivityTeacherCoverList_SelectOnly.sql"/>
+    <s v="026.002_Dim9ScheduledActivityTeacherCoverList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="259"/>
+    <s v="Dim9ScheduledActivityRoomList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityRoomList;"/>
+    <s v="026.003_Dim9ScheduledActivityRoomList_SelectOnly.sql"/>
+    <s v="026.003_Dim9ScheduledActivityRoomList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="260"/>
+    <s v="Dim9ScheduledActivityAddressList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityAddressList;"/>
+    <s v="026.004_Dim9ScheduledActivityAddressList_SelectOnly.sql"/>
+    <s v="026.004_Dim9ScheduledActivityAddressList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="261"/>
+    <s v="Dim9ScheduledActivityStudentList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityStudentList;"/>
+    <s v="026.005_Dim9ScheduledActivityStudentList_SelectOnly.sql"/>
+    <s v="026.005_Dim9ScheduledActivityStudentList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="262"/>
+    <s v="Dim9ScheduledActivityTeachingGroupList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityTeachingGroupList;"/>
+    <s v="026.006_Dim9ScheduledActivityTeachingGroupList_SelectOnly.sql"/>
+    <s v="026.006_Dim9ScheduledActivityTeachingGroupList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="263"/>
+    <s v="Dim9ScheduledActivityYearLevels"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityYearLevels;"/>
+    <s v="026.007_Dim9ScheduledActivityYearLevels_SelectOnly.sql"/>
+    <s v="026.007_Dim9ScheduledActivityYearLevels_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="264"/>
+    <s v="Dim9ScheduledActivityChangeReasonList"/>
+    <m/>
+    <x v="26"/>
+    <x v="26"/>
+    <s v="SELECT * FROM cdm_demo_gold.Dim9ScheduledActivityChangeReasonList;"/>
+    <s v="026.008_Dim9ScheduledActivityChangeReasonList_SelectOnly.sql"/>
+    <s v="026.008_Dim9ScheduledActivityChangeReasonList_InsertData.sql"/>
+  </r>
+  <r>
+    <n v="265"/>
+    <s v="Fact9ResourceBooking"/>
+    <m/>
+    <x v="27"/>
+    <x v="27"/>
+    <s v="SELECT * FROM cdm_demo_gold.Fact9ResourceBooking;"/>
+    <s v="027.001_Fact9ResourceBooking_SelectOnly.sql"/>
+    <s v="027.001_Fact9ResourceBooking_InsertData.sql"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ED1DD9D9-82B3-41CF-817B-7BCDAADCB0D5}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="127" compact="0" compactData="0" multipleFieldFilters="0" customListSort="0">
+  <location ref="A1:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="8">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="28">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="28">
+        <item sd="0" x="1"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="22"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="28">
+    <i>
+      <x/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="13"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="14"/>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="15"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="16"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="17"/>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="18"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="19"/>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="20"/>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="22"/>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="23"/>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="24"/>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="25"/>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="26"/>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="27"/>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1331,8 +4296,8 @@
   <dimension ref="A1:H266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E266"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8550,6 +11515,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H266" xr:uid="{3C96DAAC-E729-43AC-8F52-A119C0FEDE41}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F266">
     <sortCondition ref="D248:D266"/>
   </sortState>
@@ -8558,4 +11524,367 @@
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K00AEFF IN-CONFIDENCE</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A64125-C57D-4CD0-9738-A2828DC0F112}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"-- "&amp;B2&amp;":"</f>
+        <v>-- Tables populated by SIF specification:</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C29" si="0">"-- "&amp;B3&amp;":"</f>
+        <v>-- eMinerva sourced reference data:</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"-- "&amp;B4&amp;" tables:"</f>
+        <v>-- StaffPersonal tables:</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" ref="C5:C29" si="1">"-- "&amp;B5&amp;" tables:"</f>
+        <v>-- LEAInfo tables:</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>-- SchoolInfo tables:</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StudentPersonal tables:</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StudentSchoolEnrollment tables:</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StaffAssignment tables:</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StudentContactPersonal tables:</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StudentContactRelationship tables:</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>-- Party, Identity, PersonPicture &amp; PrivacyObligation(s) tables:</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>-- LearningResourcePackage tables:</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>-- LearningResource tables:</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>-- EquipmentInfo tables:</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>-- RoomInfo tables:</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>-- ResourceList tables:</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>-- LibraryPatronStatus tables:</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TermInfo tables:</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>-- SchoolCourseInfo tables:</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>-- SectionInfo tables:</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>-- StudentSectionEnrollment tables:</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TimeTable tables:</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TimeTableSubject tables:</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TeachingGroup tables:</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TimeTableCell tables:</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>-- TimeTableContainer tables:</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>-- ScheduledActivity tables:</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>-- ResourceBooking tables:</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>